<commit_message>
Updated BOM and chasis drawing
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0CBEE5-1F3F-4878-A18E-9EAF253C9052}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B529C-62D1-4DB9-A054-435256B1545A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
   <si>
     <t>Part Number</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Omni</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,25 +674,25 @@
         <v>20</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>86</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G11" si="0">F4*0.00220462</f>
+        <f t="shared" ref="G4:G12" si="0">F4*0.00220462</f>
         <v>0.18959732000000001</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H11" si="1">G4*E4</f>
-        <v>0.75838928000000005</v>
+        <f t="shared" ref="H4:H12" si="1">G4*E4</f>
+        <v>0.37919464000000003</v>
       </c>
       <c r="I4" s="2">
         <v>14.99</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" ref="J4:J11" si="2">E4*I4</f>
-        <v>59.96</v>
+        <f t="shared" ref="J4:J12" si="2">E4*I4</f>
+        <v>29.98</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -792,617 +795,616 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8">
-        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>106.3107</v>
+      </c>
+      <c r="G8" s="2">
+        <f>F8*0.00220462</f>
+        <v>0.234374695434</v>
+      </c>
+      <c r="H8" s="2">
+        <f>G8*E8</f>
+        <v>0.46874939086799999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="J8" s="2">
+        <f>E8*I8</f>
+        <v>19.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>577</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>1.2720657399999999</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="1"/>
         <v>1.2720657399999999</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="2">
         <v>4.3</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J9" s="2">
         <f t="shared" si="2"/>
         <v>4.3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>266</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0.58642892000000002</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <f t="shared" si="1"/>
         <v>1.17285784</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <v>4.59</v>
       </c>
-      <c r="J9" s="2">
-        <f>E9*I9</f>
+      <c r="J10" s="2">
+        <f>E10*I10</f>
         <v>9.18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>30</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>6.6138600000000006E-2</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>0.26455440000000002</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="J10" s="2">
-        <f>E10*I10</f>
+      <c r="J11" s="2">
+        <f>E11*I11</f>
         <v>9.0399999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>4</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>92</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>0.20282504000000001</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>0.81130016000000005</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="2">
         <v>6.99</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J12" s="2">
         <f t="shared" si="2"/>
         <v>27.96</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="2">
-        <f ca="1">SUM(H3:H14)</f>
-        <v>5.6015866807999997</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2">
-        <f ca="1">SUM(J3:J14)</f>
-        <v>163.54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="H14" s="2">
+        <f>SUM(H3:H12)</f>
+        <v>5.691141431668</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2">
+        <f>SUM(J3:J12)</f>
+        <v>153.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>243</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.53</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>0.53</v>
       </c>
-      <c r="I17">
-        <v>2.5</v>
-      </c>
-      <c r="J17">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18">
+      <c r="I18">
+        <v>2.5</v>
+      </c>
+      <c r="J18">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>265</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I18">
-        <v>2.5</v>
-      </c>
-      <c r="J18">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19">
+      <c r="I19">
+        <v>2.5</v>
+      </c>
+      <c r="J19">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>243</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>0.53</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>0.53</v>
       </c>
-      <c r="I19">
-        <v>2.5</v>
-      </c>
-      <c r="J19">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20">
+      <c r="I20">
+        <v>2.5</v>
+      </c>
+      <c r="J20">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B21">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>228</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>0.5</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>0.5</v>
       </c>
-      <c r="I20">
-        <v>2.5</v>
-      </c>
-      <c r="J20">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21">
+      <c r="I21">
+        <v>2.5</v>
+      </c>
+      <c r="J21">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B22">
         <v>5</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>243</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>0.53</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>0.53</v>
       </c>
-      <c r="I21">
-        <v>2.5</v>
-      </c>
-      <c r="J21">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22">
+      <c r="I22">
+        <v>2.5</v>
+      </c>
+      <c r="J22">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B23">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>29</v>
       </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>265</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I22">
-        <v>2.5</v>
-      </c>
-      <c r="J22">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23">
+      <c r="I23">
+        <v>2.5</v>
+      </c>
+      <c r="J23">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24">
         <v>7</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>243</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>0.53</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>0.53</v>
       </c>
-      <c r="I23">
-        <v>2.5</v>
-      </c>
-      <c r="J23">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24">
+      <c r="I24">
+        <v>2.5</v>
+      </c>
+      <c r="J24">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B25">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
         <v>228</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>0.5</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>0.5</v>
       </c>
-      <c r="I24">
-        <v>2.5</v>
-      </c>
-      <c r="J24">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25">
+      <c r="I25">
+        <v>2.5</v>
+      </c>
+      <c r="J25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>32</v>
       </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25">
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26">
         <v>2</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>188</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>0.41</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>0.82</v>
       </c>
-      <c r="I25">
-        <v>2.5</v>
-      </c>
-      <c r="J25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>552</v>
-      </c>
-      <c r="G26">
-        <v>1.21</v>
-      </c>
-      <c r="H26">
-        <v>1.21</v>
-      </c>
       <c r="I26">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="J26">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>322</v>
+        <v>552</v>
       </c>
       <c r="G27">
-        <v>0.71</v>
+        <v>1.21</v>
       </c>
       <c r="H27">
-        <v>1.42</v>
+        <v>1.21</v>
       </c>
       <c r="I27">
         <v>5</v>
       </c>
       <c r="J27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>322</v>
+      </c>
+      <c r="G28">
+        <v>0.71</v>
+      </c>
+      <c r="H28">
+        <v>1.42</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>12</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>180</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>0.4</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>0.4</v>
       </c>
-      <c r="I28">
-        <v>2.5</v>
-      </c>
-      <c r="J28">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29">
+      <c r="I29">
+        <v>2.5</v>
+      </c>
+      <c r="J29">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B30">
         <v>13</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="G29">
-        <v>0.02</v>
-      </c>
-      <c r="H29">
-        <v>0.04</v>
-      </c>
-      <c r="I29">
-        <v>5.99</v>
-      </c>
-      <c r="J29">
-        <v>11.98</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30">
-        <v>86</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="G30">
-        <v>0.19</v>
+        <v>0.02</v>
       </c>
       <c r="H30">
-        <v>0.38</v>
+        <v>0.04</v>
       </c>
       <c r="I30">
-        <v>14.99</v>
+        <v>5.99</v>
       </c>
       <c r="J30">
-        <v>29.98</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+        <v>11.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31">
-        <v>7.07</v>
+        <v>86</v>
       </c>
       <c r="G31">
-        <v>0.01</v>
+        <v>0.19</v>
       </c>
       <c r="H31">
-        <v>0.02</v>
+        <v>0.38</v>
       </c>
       <c r="I31">
-        <v>4.99</v>
+        <v>14.99</v>
       </c>
       <c r="J31">
-        <v>9.98</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32">
-        <v>37.200000000000003</v>
+        <v>7.07</v>
       </c>
       <c r="G32">
-        <v>0.08</v>
+        <v>0.01</v>
       </c>
       <c r="H32">
-        <v>0.16</v>
+        <v>0.02</v>
       </c>
       <c r="I32">
         <v>4.99</v>
@@ -1413,145 +1415,145 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="F33">
-        <v>35</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="G33">
-        <v>7.8E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H33">
-        <v>0.156</v>
+        <v>0.16</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>4.99</v>
       </c>
       <c r="J33">
-        <v>2</v>
+        <v>9.98</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B34">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F34">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G34">
-        <v>6.6000000000000003E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="H34">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="I34" t="s">
-        <v>43</v>
+        <v>0.156</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
       </c>
       <c r="J34">
-        <v>4.58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B35">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>30</v>
+      </c>
+      <c r="G35">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="H35">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="I35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B36">
         <v>19</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>44</v>
       </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35">
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36">
         <v>2</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>26.9</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>0.11799999999999999</v>
       </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G37" s="2" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H37" s="2">
-        <f>SUM(H17:H35)</f>
+      <c r="H38" s="2">
+        <f>SUM(H18:H36)</f>
         <v>9.2680000000000007</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2">
-        <f>SUM(J17:J35)</f>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2">
+        <f>SUM(J18:J36)</f>
         <v>113.00000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>55</v>
-      </c>
-      <c r="G40">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="H40">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="I40">
-        <v>2.5</v>
-      </c>
-      <c r="J40">
-        <v>2.5</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -1563,27 +1565,27 @@
         <v>55</v>
       </c>
       <c r="G41">
-        <v>1.4999999999999999E-2</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="H41">
-        <v>1.4999999999999999E-2</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="I41">
         <v>2.5</v>
       </c>
       <c r="J41">
-        <v>1.75</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1592,27 +1594,27 @@
         <v>55</v>
       </c>
       <c r="G42">
-        <v>0.436</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H42">
-        <v>0.436</v>
-      </c>
-      <c r="I42" t="s">
-        <v>51</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I42">
+        <v>2.5</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1621,24 +1623,24 @@
         <v>55</v>
       </c>
       <c r="G43">
-        <v>0.58599999999999997</v>
+        <v>0.436</v>
       </c>
       <c r="H43">
-        <v>0.58599999999999997</v>
-      </c>
-      <c r="I43">
-        <v>2.5</v>
+        <v>0.436</v>
+      </c>
+      <c r="I43" t="s">
+        <v>51</v>
       </c>
       <c r="J43">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -1650,24 +1652,24 @@
         <v>55</v>
       </c>
       <c r="G44">
-        <v>0.01</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="H44">
-        <v>0.01</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="I44">
-        <v>4.99</v>
+        <v>2.5</v>
       </c>
       <c r="J44">
-        <v>4.99</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -1679,27 +1681,27 @@
         <v>55</v>
       </c>
       <c r="G45">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H45">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I45">
-        <v>5.99</v>
+        <v>4.99</v>
       </c>
       <c r="J45">
-        <v>5.99</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1708,153 +1710,156 @@
         <v>55</v>
       </c>
       <c r="G46">
-        <v>21</v>
+        <v>0.02</v>
       </c>
       <c r="H46">
-        <v>21</v>
+        <v>0.02</v>
       </c>
       <c r="I46">
-        <v>14.99</v>
+        <v>5.99</v>
       </c>
       <c r="J46">
-        <v>14.99</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
         <v>55</v>
       </c>
       <c r="G47">
+        <v>21</v>
+      </c>
+      <c r="H47">
+        <v>21</v>
+      </c>
+      <c r="I47">
+        <v>14.99</v>
+      </c>
+      <c r="J47">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48">
         <v>7.8E-2</v>
       </c>
-      <c r="H47">
+      <c r="H48">
         <v>0.23400000000000001</v>
       </c>
-      <c r="I47">
-        <v>1</v>
-      </c>
-      <c r="J47">
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G49" s="2" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G50" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H49" s="2">
-        <f>SUM(H40:H47)</f>
+      <c r="H50" s="2">
+        <f>SUM(H41:H48)</f>
         <v>22.87</v>
       </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2">
-        <f>SUM(J40:J47)</f>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2">
+        <f>SUM(J41:J48)</f>
         <v>36.72</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" t="s">
-        <v>54</v>
-      </c>
-      <c r="E52">
-        <v>2</v>
-      </c>
-      <c r="F52" t="s">
-        <v>55</v>
-      </c>
-      <c r="G52">
-        <v>0.25</v>
-      </c>
-      <c r="H52">
-        <v>0.5</v>
-      </c>
-      <c r="I52" t="s">
-        <v>58</v>
-      </c>
-      <c r="J52">
-        <v>15.98</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" t="s">
         <v>55</v>
       </c>
       <c r="G53">
-        <v>2.36</v>
+        <v>0.25</v>
       </c>
       <c r="H53">
-        <v>2.36</v>
+        <v>0.5</v>
       </c>
       <c r="I53" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J53">
-        <v>14.99</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="E54">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="F54" t="s">
         <v>55</v>
       </c>
       <c r="G54">
-        <v>1.42</v>
+        <v>2.36</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>2.36</v>
       </c>
       <c r="I54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J54">
-        <v>22.98</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D55" t="s">
         <v>73</v>
       </c>
       <c r="E55">
-        <v>0.82</v>
+        <v>1.4</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
@@ -1863,7 +1868,7 @@
         <v>1.42</v>
       </c>
       <c r="H55">
-        <v>1.17</v>
+        <v>2</v>
       </c>
       <c r="I55" t="s">
         <v>62</v>
@@ -1874,13 +1879,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D56" t="s">
         <v>73</v>
       </c>
       <c r="E56">
-        <v>0.63</v>
+        <v>0.82</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
@@ -1889,7 +1894,7 @@
         <v>1.42</v>
       </c>
       <c r="H56">
-        <v>0.89</v>
+        <v>1.17</v>
       </c>
       <c r="I56" t="s">
         <v>62</v>
@@ -1900,116 +1905,142 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D57" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>0.63</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
       </c>
       <c r="G57">
-        <v>7.0000000000000007E-2</v>
+        <v>1.42</v>
       </c>
       <c r="H57">
-        <v>0.27</v>
+        <v>0.89</v>
       </c>
       <c r="I57" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J57">
-        <v>5.3</v>
+        <v>22.98</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="D58" t="s">
+        <v>18</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F58" t="s">
         <v>55</v>
       </c>
       <c r="G58">
-        <v>0.5</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0.27</v>
       </c>
       <c r="I58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J58">
-        <v>5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
         <v>55</v>
       </c>
       <c r="G59">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H59">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J59">
-        <v>7.56</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
       </c>
       <c r="E60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
       </c>
       <c r="G60">
+        <v>0.4</v>
+      </c>
+      <c r="H60">
+        <v>1.6</v>
+      </c>
+      <c r="I60" t="s">
+        <v>70</v>
+      </c>
+      <c r="J60">
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
         <v>0</v>
       </c>
-      <c r="H60">
+      <c r="H61">
         <v>0</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I61" t="s">
         <v>72</v>
       </c>
-      <c r="J60">
+      <c r="J61">
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G62" s="2" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G63" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H62" s="2">
-        <f>SUM(H52:H60)</f>
+      <c r="H63" s="2">
+        <f>SUM(H53:H61)</f>
         <v>9.7899999999999991</v>
       </c>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2">
-        <f>SUM(J52:J60)</f>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2">
+        <f>SUM(J53:J61)</f>
         <v>127.31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Meeting, nothing actually changed
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94B529C-62D1-4DB9-A054-435256B1545A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6D5AFA-7554-487A-96BC-ABAF431EA9AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7">
-        <f t="shared" ref="B7:B11" si="3">B6+1</f>
+        <f t="shared" ref="B7" si="3">B6+1</f>
         <v>5</v>
       </c>
       <c r="C7" t="s">

</xml_diff>